<commit_message>
Customer, Vendor Sample file chgs
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/customer.xlsx
+++ b/src/assets/sample-files/customer.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\finance-frontend\src\assets\sample-files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Customer Name</t>
   </si>
@@ -116,18 +121,9 @@
     <t>TN</t>
   </si>
   <si>
-    <t>dfn</t>
-  </si>
-  <si>
-    <t>Mettur</t>
-  </si>
-  <si>
     <t>Commericial</t>
   </si>
   <si>
-    <t>Mecheri</t>
-  </si>
-  <si>
     <t>State No</t>
   </si>
   <si>
@@ -143,12 +139,6 @@
     <t>TN000001</t>
   </si>
   <si>
-    <t>HARI</t>
-  </si>
-  <si>
-    <t>hari@gmail.com</t>
-  </si>
-  <si>
     <t>MANUFACTURER</t>
   </si>
   <si>
@@ -161,31 +151,55 @@
     <t>CHENNAI</t>
   </si>
   <si>
-    <t>PRABHU</t>
-  </si>
-  <si>
     <t>BENGALURU</t>
   </si>
   <si>
     <t>Gst In</t>
   </si>
   <si>
-    <t>TN0</t>
-  </si>
-  <si>
     <t>WDS010</t>
   </si>
   <si>
-    <t>NARASIMHA</t>
-  </si>
-  <si>
-    <t>DHINESHKUMAR1</t>
+    <t>29GGGGG1314R9Z6</t>
+  </si>
+  <si>
+    <t>ABCDE1234F</t>
+  </si>
+  <si>
+    <t>ABCD PVT LTD</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Defg</t>
+  </si>
+  <si>
+    <t>Hij</t>
+  </si>
+  <si>
+    <t>JOE</t>
+  </si>
+  <si>
+    <t>ALICE</t>
+  </si>
+  <si>
+    <t>joe@gmail.com</t>
+  </si>
+  <si>
+    <t>alice@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
@@ -227,12 +241,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -294,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,17 +554,17 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -564,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -596,13 +609,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -611,19 +624,19 @@
         <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>43</v>
-      </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
         <v>30</v>
@@ -639,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +676,7 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -683,7 +696,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>31</v>
@@ -692,24 +705,24 @@
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2">
-        <v>9080887678</v>
+        <v>9876543210</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>31</v>
@@ -718,19 +731,19 @@
         <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F3" s="2">
-        <v>9080887678</v>
+        <v>9876543210</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -748,14 +761,14 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -801,72 +814,72 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="I2">
-        <v>560106</v>
+        <v>100001</v>
       </c>
       <c r="J2">
-        <v>9080335965</v>
+        <v>9876543210</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="I3">
-        <v>560106</v>
+        <v>100001</v>
       </c>
       <c r="J3">
-        <v>9080335965</v>
+        <v>9876543210</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -876,10 +889,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,35 +905,55 @@
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="D2" s="1">
+        <v>46016</v>
+      </c>
+      <c r="E2" s="1">
+        <v>46017</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1">
         <v>46016</v>
@@ -929,27 +962,7 @@
         <v>46017</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="1">
-        <v>46016</v>
-      </c>
-      <c r="E4" s="1">
-        <v>46017</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -959,10 +972,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,11 +997,8 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>